<commit_message>
add geopy to src and try debug main.py
</commit_message>
<xml_diff>
--- a/src/databases/safety_factors.xlsx
+++ b/src/databases/safety_factors.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="port_sf" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Terminal dock size area (m²)</t>
   </si>
@@ -584,7 +584,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,9 +819,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="1" t="s">
         <v>22</v>

</xml_diff>